<commit_message>
Check_list_Exporer.xlsx has been fixed
</commit_message>
<xml_diff>
--- a/Check_list_MSG.xlsx
+++ b/Check_list_MSG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bezus\Desktop\Дима\Дима, для работы\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7770F8C1-3F91-4B6E-AC55-8A4F5E1F10C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10387BAC-428C-493D-884C-6FEC05002F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="11904" xr2:uid="{AB52E13C-34F1-4F78-B52D-9AB426BDCDB6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="123">
   <si>
     <t>Проверка</t>
   </si>
@@ -324,12 +324,129 @@
       <t xml:space="preserve"> от окна сообщения</t>
     </r>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>MSG.1.1</t>
+  </si>
+  <si>
+    <t>MSG.1.2</t>
+  </si>
+  <si>
+    <t>MSG.1.3</t>
+  </si>
+  <si>
+    <t>MSG.1.4</t>
+  </si>
+  <si>
+    <t>MSG.1.5</t>
+  </si>
+  <si>
+    <t>MSG.1.6</t>
+  </si>
+  <si>
+    <t>MSG.2.1</t>
+  </si>
+  <si>
+    <t>MSG.2.2</t>
+  </si>
+  <si>
+    <t>MSG.2.3</t>
+  </si>
+  <si>
+    <t>MSG.2.4</t>
+  </si>
+  <si>
+    <t>MSG.3.1.1</t>
+  </si>
+  <si>
+    <t>MSG.3.1.2</t>
+  </si>
+  <si>
+    <t>MSG.3.1.3</t>
+  </si>
+  <si>
+    <t>MSG.3.1.4</t>
+  </si>
+  <si>
+    <t>MSG.3.1.5</t>
+  </si>
+  <si>
+    <t>MSG.3.1.6</t>
+  </si>
+  <si>
+    <t>MSG.3.1.7</t>
+  </si>
+  <si>
+    <t>MSG.3.1.8</t>
+  </si>
+  <si>
+    <t>MSG.3.1.9</t>
+  </si>
+  <si>
+    <t>MSG.3.2.1</t>
+  </si>
+  <si>
+    <t>MSG.3.2.2</t>
+  </si>
+  <si>
+    <t>MSG.3.2.3</t>
+  </si>
+  <si>
+    <t>MSG.3.2.4</t>
+  </si>
+  <si>
+    <t>MSG.3.2.5</t>
+  </si>
+  <si>
+    <t>MSG.3.3.1</t>
+  </si>
+  <si>
+    <t>MSG.3.3.2</t>
+  </si>
+  <si>
+    <t>MSG.3.4.1</t>
+  </si>
+  <si>
+    <t>MSG.3.4.2</t>
+  </si>
+  <si>
+    <t>MSG.3.4.3</t>
+  </si>
+  <si>
+    <t>MSG.3.4.4</t>
+  </si>
+  <si>
+    <t>MSG.3.4.5</t>
+  </si>
+  <si>
+    <t>MSG.3.4.6</t>
+  </si>
+  <si>
+    <t>MSG.3.4.7</t>
+  </si>
+  <si>
+    <t>MSG.3.4.8</t>
+  </si>
+  <si>
+    <t>MSG.3.4.9</t>
+  </si>
+  <si>
+    <t>MSG.3.4.10</t>
+  </si>
+  <si>
+    <t>MSG.3.4.11</t>
+  </si>
+  <si>
+    <t>MSG.3.4.12</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,8 +476,15 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +524,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -485,9 +621,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -496,6 +629,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -817,507 +959,634 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51070EE9-4B7C-4610-B74A-B1C86B0D62AA}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.88671875" customWidth="1"/>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
-    <col min="3" max="3" width="50.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="55.77734375" customWidth="1"/>
+    <col min="3" max="3" width="55.109375" customWidth="1"/>
+    <col min="4" max="4" width="55.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A2" s="16"/>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="13"/>
-    </row>
-    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="13"/>
-    </row>
-    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="13"/>
-    </row>
-    <row r="6" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="13"/>
-    </row>
-    <row r="7" spans="1:3" ht="36" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="D6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="D7" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="D8" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="D12" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="D13" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A14" s="16"/>
+      <c r="B14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="D17" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="D18" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="D20" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="D21" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="D23" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="D25" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A26" s="16"/>
+      <c r="B26" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="14"/>
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="C26" s="13"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="D29" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+    <row r="30" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="D31" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A32" s="16"/>
+      <c r="B32" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="3"/>
       <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="D33" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="A34" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A35" s="8" t="s">
+    <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A35" s="16"/>
+      <c r="B35" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="3"/>
       <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
+      <c r="D36" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="D37" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
+      <c r="D38" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>37</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+      <c r="D39" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A40" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A41" s="12" t="s">
+      <c r="D40" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A41" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>77</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="D41" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A42" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="D42" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="36" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
+    <row r="43" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+      <c r="A43" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="D43" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A44" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D44" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+    <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A45" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="36" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+      <c r="D45" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+      <c r="A46" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="D46" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="54" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="A47" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="D47" s="14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A48" s="3"/>
-      <c r="B48" s="3"/>
-      <c r="C48" s="3"/>
+    <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+      <c r="A48" s="17"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
     </row>
     <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Check_list_MSG.xlsx has been fixed and msg_test_cases.xls.xlsx was added
</commit_message>
<xml_diff>
--- a/Check_list_MSG.xlsx
+++ b/Check_list_MSG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10387BAC-428C-493D-884C-6FEC05002F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B5F3156-7BE8-4AE8-9935-9F9FF0E0ABFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="11904" xr2:uid="{AB52E13C-34F1-4F78-B52D-9AB426BDCDB6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="126">
   <si>
     <t>Проверка</t>
   </si>
@@ -440,6 +440,15 @@
   </si>
   <si>
     <t>MSG.3.4.12</t>
+  </si>
+  <si>
+    <t>MSG.3.4.13</t>
+  </si>
+  <si>
+    <t>Удаление отправленных сообщений</t>
+  </si>
+  <si>
+    <t>Сообщение удалено</t>
   </si>
 </sst>
 </file>
@@ -591,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -637,8 +646,11 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51070EE9-4B7C-4610-B74A-B1C86B0D62AA}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1534,51 +1546,60 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>43</v>
+      <c r="B45" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="36" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>44</v>
+      <c r="B46" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="36" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>122</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="54" x14ac:dyDescent="0.3">
+      <c r="A48" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D48" s="14" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A48" s="17"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
     </row>
     <row r="49" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A49" s="17"/>

</xml_diff>